<commit_message>
Modifying the entity draw
</commit_message>
<xml_diff>
--- a/documents/anicas-store.xlsx
+++ b/documents/anicas-store.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\CsvLoader\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52E70BB1-796B-44F6-B5B2-E5565280FCBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A30B3C61-1417-4FC3-8936-A859F3E45118}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -369,7 +369,7 @@
   <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>